<commit_message>
Arranging PCO density matrix correctly and rerun entire code. Updated PCO figures and PERMANOVA tables.
</commit_message>
<xml_diff>
--- a/Tables/BETADISPERSION_PCO_biomass_bioreg.xlsx
+++ b/Tables/BETADISPERSION_PCO_biomass_bioreg.xlsx
@@ -115,19 +115,19 @@
         <v>3.0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4700963020062678</v>
+        <v>0.44115549721919844</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1566987673354226</v>
+        <v>0.1470518324063995</v>
       </c>
       <c r="E2" t="n">
-        <v>6.07510838721917</v>
+        <v>4.884781506196352</v>
       </c>
       <c r="F2" t="n">
         <v>9999.0</v>
       </c>
       <c r="G2" t="n">
-        <v>4.0E-4</v>
+        <v>0.0041</v>
       </c>
     </row>
     <row r="3">
@@ -138,10 +138,10 @@
         <v>144.0</v>
       </c>
       <c r="C3" t="n">
-        <v>3.714274883353912</v>
+        <v>4.334986905690751</v>
       </c>
       <c r="D3" t="n">
-        <v>0.02579357557884661</v>
+        <v>0.030104075733963547</v>
       </c>
       <c r="E3" t="e">
         <v>#N/A</v>

</xml_diff>

<commit_message>
Tables remade due to rerun of calculations, p-values changes slightly due to permutations so new tables are saved.
</commit_message>
<xml_diff>
--- a/Tables/BETADISPERSION_PCO_biomass_bioreg.xlsx
+++ b/Tables/BETADISPERSION_PCO_biomass_bioreg.xlsx
@@ -386,19 +386,19 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>0.442692287059714</v>
+        <v>0.536887325674664</v>
       </c>
       <c r="C2" t="n">
-        <v>0.147564095686571</v>
+        <v>0.178962441891555</v>
       </c>
       <c r="D2" t="n">
-        <v>4.90897651908444</v>
+        <v>8.67387631321838</v>
       </c>
       <c r="E2" t="n">
         <v>9999</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0032</v>
+        <v>0.0001</v>
       </c>
     </row>
     <row r="3">
@@ -406,10 +406,10 @@
         <v>144</v>
       </c>
       <c r="B3" t="n">
-        <v>4.32864767151696</v>
+        <v>2.97105823299686</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0300600532744233</v>
+        <v>0.0206323488402559</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>

</xml_diff>